<commit_message>
it's over, it's done
</commit_message>
<xml_diff>
--- a/PythonLand/smalldataanalysis.xlsx
+++ b/PythonLand/smalldataanalysis.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3C221E38-579F-45C9-B0CC-C1DD85A872E7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6A09D904-A5DE-4197-87F1-3D1FE57B1053}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="7860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,6 +13,20 @@
   <calcPr calcId="0"/>
   <oleSize ref="A1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Genetic Algorithm</t>
+  </si>
+  <si>
+    <t>Hill Climber</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18858,7 +18872,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -20069,14 +20082,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K2000"/>
+  <dimension ref="A1:K2000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+    <sheetView tabSelected="1" topLeftCell="A976" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K1001" sqref="K1001"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>

</xml_diff>